<commit_message>
updated contact-summary and tasks
</commit_message>
<xml_diff>
--- a/cht_oppia_mvp/forms/app/cha_module_one.xlsx
+++ b/cht_oppia_mvp/forms/app/cha_module_one.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="207">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -159,20 +159,28 @@
     <t xml:space="preserve">step_one</t>
   </si>
   <si>
-    <t xml:space="preserve">Step 1:
+    <t xml:space="preserve">**Step 1:**
 Open Oppia Mobile to read the course content. Once complete, please return to this task for Step 2.</t>
   </si>
   <si>
     <t xml:space="preserve">introduction</t>
   </si>
   <si>
-    <t xml:space="preserve">This first module, **Introduction to COVID-19**, explains what coronavirus disease (COVID-19) is, where it comes from, and how it spreads. You will learn how to reduce the risk of contracting and spreading COVID-19, and review information on how to protect yourself and your community. </t>
+    <t xml:space="preserve">This first module, **Introduction to COVID-19**, explains what coronavirus disease (COVID-19) is, where it comes from, and how it spreads. You will learn how to reduce the risk of contracting and spreading COVID-19, and review information on how to protect yourself and your community. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open_oppia_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[&lt;span style='background-color: #648af7; color:white; padding: 1em; text-decoration: none;border-radius: 8px; '&gt;Open Oppia Mobile&lt;/span&gt;](https://staging.cha.oppia-mobile.org/view?course=cht-demo)</t>
   </si>
   <si>
     <t xml:space="preserve">step_two</t>
   </si>
   <si>
-    <t xml:space="preserve">Step 2:
+    <t xml:space="preserve">
+**Step 2:**
 Complete a short assessment on the course material.</t>
   </si>
   <si>
@@ -822,11 +830,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -934,11 +942,11 @@
   <dimension ref="A1:BB52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="C48" activeCellId="0" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1198,7 +1206,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1220,15 +1228,26 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="55.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="8" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,10 +1260,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>19</v>
@@ -1252,229 +1271,229 @@
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="J24" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>57</v>
+        <v>80</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>57</v>
+        <v>85</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>57</v>
+        <v>90</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>57</v>
+        <v>95</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,31 +1502,31 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,13 +1534,13 @@
         <v>15</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,10 +1548,10 @@
         <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,13 +1559,13 @@
         <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,30 +1573,30 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,16 +1604,16 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,16 +1621,16 @@
         <v>43</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,50 +1638,50 @@
         <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,30 +1689,30 @@
         <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,7 +1755,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -1747,321 +1766,321 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2097,40 +2116,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C2" s="15" t="n">
         <f aca="true">NOW()</f>
-        <v>44090.0432900963</v>
+        <v>44091.7605709773</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated targets, contact summary; added context forms
</commit_message>
<xml_diff>
--- a/cht_oppia_mvp/forms/app/cha_module_one.xlsx
+++ b/cht_oppia_mvp/forms/app/cha_module_one.xlsx
@@ -217,7 +217,7 @@
     <t xml:space="preserve">asymptomatic_spread_q</t>
   </si>
   <si>
-    <t xml:space="preserve">2. A person who is infected with COVID-19, but does not have symptoms can pass the virus to another person.(single_select)</t>
+    <t xml:space="preserve">2. A person who is infected with COVID-19, but does not have symptoms can pass the virus to another person.</t>
   </si>
   <si>
     <t xml:space="preserve">asymptomatic_spread_score</t>
@@ -371,7 +371,7 @@
     <t xml:space="preserve">success_note</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you for completing "Module 1: Introduction to COVID-19. You **scored ${assessment_score}** out of 8. Great Job, you’ve completed Module 1! You can revisit this content at any time in your Oppia app.</t>
+    <t xml:space="preserve">Great Job! You’ve completed Module 1: Introduction to COVID-19! You can revisit this content at any time in your Oppia app.</t>
   </si>
   <si>
     <t xml:space="preserve">${assessment_passed} = ‘yes’</t>
@@ -942,11 +942,11 @@
   <dimension ref="A1:BB52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="bottomRight" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1599,7 +1599,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="C2" s="15" t="n">
         <f aca="true">NOW()</f>
-        <v>44091.7605709773</v>
+        <v>44105.6656556913</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>205</v>

</xml_diff>